<commit_message>
update contents of VCHAINS dir
</commit_message>
<xml_diff>
--- a/nlp/data/VCHAINS/4295915260_VCHAINS.xlsx
+++ b/nlp/data/VCHAINS/4295915260_VCHAINS.xlsx
@@ -14,16 +14,16 @@
     <x:definedName name="CriteriaLabels">'Value Chains'!$A$3:$A$4</x:definedName>
     <x:definedName name="CriteriaValues">'Value Chains'!$B$3:$B$4</x:definedName>
     <x:definedName name="ColumnHeader">'Value Chains'!$A$6:$N$6</x:definedName>
-    <x:definedName name="Data">'Value Chains'!$A$7:$N$11</x:definedName>
-    <x:definedName name="DataConfidenceScore">'Value Chains'!$G$7:$G$11</x:definedName>
-    <x:definedName name="DataRevenue">'Value Chains'!$I$7:$I$11</x:definedName>
+    <x:definedName name="Data">'Value Chains'!$A$7:$N$29</x:definedName>
+    <x:definedName name="DataConfidenceScore">'Value Chains'!$G$7:$G$29</x:definedName>
+    <x:definedName name="DataRevenue">'Value Chains'!$I$7:$I$29</x:definedName>
   </x:definedNames>
   <x:calcPr calcId="125725"/>
 </x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <x:si>
     <x:t>Value Chains</x:t>
   </x:si>
@@ -31,7 +31,7 @@
     <x:t>Company Name</x:t>
   </x:si>
   <x:si>
-    <x:t>Lite-On Technology Corp</x:t>
+    <x:t>Universal Display Corp</x:t>
   </x:si>
   <x:si>
     <x:t>Company Id</x:t>
@@ -76,55 +76,163 @@
     <x:t>Implied Rating</x:t>
   </x:si>
   <x:si>
+    <x:t>Samsung Electronics Co Ltd</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Public</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Customer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Korea; Republic (S. Korea)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Phones &amp; Handheld Devices</x:t>
+  </x:si>
+  <x:si>
+    <x:t>A+</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PPG Industries Inc</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Supplier</x:t>
+  </x:si>
+  <x:si>
+    <x:t>United States of America</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Commodity Chemicals</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LG Display Co Ltd</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Electronic Equipment &amp; Parts</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Systems Design Co Ltd</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Japan</x:t>
+  </x:si>
+  <x:si>
+    <x:t>IT Services &amp; Consulting</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AA-</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Samsung Display Co Ltd</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Private</x:t>
+  </x:si>
+  <x:si>
     <x:t>Apple Inc</x:t>
   </x:si>
   <x:si>
-    <x:t>Public</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Customer</x:t>
-  </x:si>
-  <x:si>
-    <x:t>United States of America</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Phones &amp; Handheld Devices</x:t>
-  </x:si>
-  <x:si>
     <x:t>A</x:t>
   </x:si>
   <x:si>
-    <x:t>Roku Inc</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Supplier</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Entertainment Production</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Cypress Semiconductor Corp</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Private</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Semiconductors</x:t>
+    <x:t>AU Optronics Corp</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Taiwan</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Lumiotec Inc</x:t>
+  </x:si>
+  <x:si>
+    <x:t>-</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Motorola Solutions Inc</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Communications &amp; Networking</x:t>
+  </x:si>
+  <x:si>
+    <x:t>B+</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LG Chem Ltd</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BBB+</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Tianma Microelectronics Co Ltd</x:t>
+  </x:si>
+  <x:si>
+    <x:t>China</x:t>
   </x:si>
   <x:si>
     <x:t>BBB-</x:t>
   </x:si>
   <x:si>
-    <x:t>Optomec Inc</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Electronic Equipment &amp; Parts</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Kioxia Holdings Corp</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Japan</x:t>
+    <x:t>Konica Minolta Inc</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Office Equipment</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Innolux Corp</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Moser Baer Technologies Inc</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Aixtron AG</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Germany</x:t>
+  </x:si>
+  <x:si>
+    <x:t>EPIGRESS AB(AIXTRON AG)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Sweden</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SDC Investimentos SA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Portugal</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Highways &amp; Rail Tracks</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Idemitsu Kosan Co Ltd</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Oil &amp; Gas Refining and Marketing</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Panasonic Corp</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Household Electronics</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Visionox Technology Inc</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PolarityTE Inc</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Biotechnology &amp; Medical Research</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Oledworks LLC</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Electrical Components &amp; Equipment</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -578,24 +686,24 @@
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
     <x:pageSetUpPr fitToPage="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:N11"/>
+  <x:dimension ref="A1:N29"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
     <x:col min="1" max="1" width="15.700625" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="26.300625" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="28.720625000000002" style="0" customWidth="1"/>
     <x:col min="3" max="3" width="7.830625" style="0" customWidth="1"/>
     <x:col min="4" max="4" width="12.710625" style="0" customWidth="1"/>
-    <x:col min="5" max="5" width="23.040625" style="0" customWidth="1"/>
-    <x:col min="6" max="6" width="26.790625" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="23.850625" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="32.600625" style="0" customWidth="1"/>
     <x:col min="7" max="7" width="20.190625" style="0" customWidth="1"/>
     <x:col min="8" max="8" width="16.840625000000003" style="0" customWidth="1"/>
     <x:col min="9" max="9" width="21.920625" style="0" customWidth="1"/>
     <x:col min="10" max="10" width="10.410625" style="0" customWidth="1"/>
     <x:col min="11" max="11" width="14.180625000000001" style="0" customWidth="1"/>
-    <x:col min="12" max="12" width="14.880625" style="0" customWidth="1"/>
+    <x:col min="12" max="12" width="18.300625" style="0" customWidth="1"/>
     <x:col min="13" max="13" width="9.570625" style="0" customWidth="1"/>
     <x:col min="14" max="14" width="14.480625" style="0" customWidth="1"/>
   </x:cols>
@@ -605,7 +713,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="B1" s="2">
-        <x:v>44595.9236111111</x:v>
+        <x:v>44596.3145833333</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:14" customFormat="1" ht="32.26" customHeight="1">
@@ -639,7 +747,7 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="B4" s="5" t="n">
-        <x:v>4295891508</x:v>
+        <x:v>4295915260</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:14">
@@ -688,7 +796,7 @@
     </x:row>
     <x:row r="7" spans="1:14">
       <x:c r="A7" s="5" t="n">
-        <x:v>4295905573</x:v>
+        <x:v>4295882451</x:v>
       </x:c>
       <x:c r="B7" s="5" t="s">
         <x:v>17</x:v>
@@ -706,25 +814,25 @@
         <x:v>21</x:v>
       </x:c>
       <x:c r="G7" s="7" t="n">
-        <x:v>1</x:v>
+        <x:v>0.998317852334147</x:v>
       </x:c>
       <x:c r="H7" s="8">
-        <x:v>43132</x:v>
+        <x:v>43685</x:v>
       </x:c>
       <x:c r="I7" s="9" t="n">
-        <x:v>1463</x:v>
+        <x:v>911</x:v>
       </x:c>
       <x:c r="J7" s="5" t="n">
-        <x:v>2</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="K7" s="5" t="n">
-        <x:v>1</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="L7" s="5" t="n">
-        <x:v>365817000000</x:v>
+        <x:v>243974550248.924</x:v>
       </x:c>
       <x:c r="M7" s="5" t="n">
-        <x:v>80</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="N7" s="5" t="s">
         <x:v>22</x:v>
@@ -732,7 +840,7 @@
     </x:row>
     <x:row r="8" spans="1:14">
       <x:c r="A8" s="5" t="n">
-        <x:v>4297900917</x:v>
+        <x:v>4295904686</x:v>
       </x:c>
       <x:c r="B8" s="5" t="s">
         <x:v>23</x:v>
@@ -744,155 +852,921 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="E8" s="5" t="s">
-        <x:v>20</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="F8" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="G8" s="7" t="n">
-        <x:v>0.55678434528</x:v>
+        <x:v>0.980136067921922</x:v>
       </x:c>
       <x:c r="H8" s="8">
-        <x:v>43062</x:v>
+        <x:v>42979</x:v>
       </x:c>
       <x:c r="I8" s="9" t="n">
-        <x:v>1533</x:v>
+        <x:v>1617</x:v>
       </x:c>
       <x:c r="J8" s="5" t="n">
-        <x:v>2</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="K8" s="5" t="n">
-        <x:v>3</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="L8" s="5" t="n">
-        <x:v>1778388000</x:v>
+        <x:v>16802000000</x:v>
       </x:c>
       <x:c r="M8" s="5" t="n">
-        <x:v>93</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="N8" s="5" t="s">
-        <x:v>22</x:v>
+        <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:14">
       <x:c r="A9" s="5" t="n">
-        <x:v>4295903116</x:v>
+        <x:v>4295882602</x:v>
       </x:c>
       <x:c r="B9" s="5" t="s">
-        <x:v>26</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="C9" s="5" t="s">
-        <x:v>27</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="D9" s="5" t="s">
-        <x:v>24</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="E9" s="5" t="s">
         <x:v>20</x:v>
       </x:c>
       <x:c r="F9" s="5" t="s">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="G9" s="7" t="n">
-        <x:v>0.30366456</x:v>
+        <x:v>0.974520097573171</x:v>
       </x:c>
       <x:c r="H9" s="8">
-        <x:v>41156</x:v>
+        <x:v>43517</x:v>
       </x:c>
       <x:c r="I9" s="9" t="n">
-        <x:v>3439</x:v>
+        <x:v>1079</x:v>
       </x:c>
       <x:c r="J9" s="5" t="n">
-        <x:v>1</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="K9" s="5" t="n">
-        <x:v>2</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="L9" s="5" t="n">
-        <x:v>2205314000</x:v>
-      </x:c>
-      <x:c r="M9" s="5" t="s"/>
+        <x:v>26127175997.2868</x:v>
+      </x:c>
+      <x:c r="M9" s="5" t="n">
+        <x:v>43</x:v>
+      </x:c>
       <x:c r="N9" s="5" t="s">
-        <x:v>29</x:v>
+        <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:14">
       <x:c r="A10" s="5" t="n">
-        <x:v>4297422171</x:v>
+        <x:v>4295876478</x:v>
       </x:c>
       <x:c r="B10" s="5" t="s">
         <x:v>30</x:v>
       </x:c>
       <x:c r="C10" s="5" t="s">
-        <x:v>27</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="D10" s="5" t="s">
-        <x:v>24</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="E10" s="5" t="s">
-        <x:v>20</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="F10" s="5" t="s">
-        <x:v>31</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="G10" s="7" t="n">
-        <x:v>0.29733864</x:v>
+        <x:v>0.970068963725295</x:v>
       </x:c>
       <x:c r="H10" s="8">
-        <x:v>42452</x:v>
+        <x:v>43405</x:v>
       </x:c>
       <x:c r="I10" s="9" t="n">
-        <x:v>2143</x:v>
+        <x:v>1191</x:v>
       </x:c>
       <x:c r="J10" s="5" t="n">
-        <x:v>1</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="K10" s="5" t="n">
-        <x:v>2</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="L10" s="5" t="n">
-        <x:v>8007154</x:v>
-      </x:c>
-      <x:c r="M10" s="5" t="s"/>
-      <x:c r="N10" s="5" t="s"/>
+        <x:v>75174031.7284788</x:v>
+      </x:c>
+      <x:c r="M10" s="5" t="n">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="N10" s="5" t="s">
+        <x:v>33</x:v>
+      </x:c>
     </x:row>
     <x:row r="11" spans="1:14">
       <x:c r="A11" s="5" t="n">
-        <x:v>5068663189</x:v>
+        <x:v>5037430729</x:v>
       </x:c>
       <x:c r="B11" s="5" t="s">
-        <x:v>32</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="C11" s="5" t="s">
-        <x:v>27</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="D11" s="5" t="s">
         <x:v>19</x:v>
       </x:c>
       <x:c r="E11" s="5" t="s">
-        <x:v>33</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="F11" s="5" t="s">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="G11" s="7" t="n">
-        <x:v>0.2897888</x:v>
+        <x:v>0.694470377470083</x:v>
       </x:c>
       <x:c r="H11" s="8">
-        <x:v>43710</x:v>
+        <x:v>43404</x:v>
       </x:c>
       <x:c r="I11" s="9" t="n">
-        <x:v>885</x:v>
+        <x:v>1192</x:v>
       </x:c>
       <x:c r="J11" s="5" t="n">
-        <x:v>4</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="K11" s="5" t="n">
-        <x:v>2</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="L11" s="5" t="s"/>
       <x:c r="M11" s="5" t="s"/>
       <x:c r="N11" s="5" t="s"/>
+    </x:row>
+    <x:row r="12" spans="1:14">
+      <x:c r="A12" s="5" t="n">
+        <x:v>4295905573</x:v>
+      </x:c>
+      <x:c r="B12" s="5" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="C12" s="5" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="D12" s="5" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="E12" s="5" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="F12" s="5" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="G12" s="7" t="n">
+        <x:v>0.642186603918336</x:v>
+      </x:c>
+      <x:c r="H12" s="8">
+        <x:v>43881</x:v>
+      </x:c>
+      <x:c r="I12" s="9" t="n">
+        <x:v>715</x:v>
+      </x:c>
+      <x:c r="J12" s="5" t="n">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="K12" s="5" t="n">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="L12" s="5" t="n">
+        <x:v>365817000000</x:v>
+      </x:c>
+      <x:c r="M12" s="5" t="n">
+        <x:v>80</x:v>
+      </x:c>
+      <x:c r="N12" s="5" t="s">
+        <x:v>37</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:14">
+      <x:c r="A13" s="5" t="n">
+        <x:v>4295890965</x:v>
+      </x:c>
+      <x:c r="B13" s="5" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="C13" s="5" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="D13" s="5" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="E13" s="5" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="F13" s="5" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="G13" s="7" t="n">
+        <x:v>0.629129792487475</x:v>
+      </x:c>
+      <x:c r="H13" s="8">
+        <x:v>43153</x:v>
+      </x:c>
+      <x:c r="I13" s="9" t="n">
+        <x:v>1443</x:v>
+      </x:c>
+      <x:c r="J13" s="5" t="n">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="K13" s="5" t="n">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="L13" s="5" t="n">
+        <x:v>9206896345.69449</x:v>
+      </x:c>
+      <x:c r="M13" s="5" t="n">
+        <x:v>94</x:v>
+      </x:c>
+      <x:c r="N13" s="5" t="s">
+        <x:v>37</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:14">
+      <x:c r="A14" s="5" t="n">
+        <x:v>4298029154</x:v>
+      </x:c>
+      <x:c r="B14" s="5" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="C14" s="5" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="D14" s="5" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="E14" s="5" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="F14" s="5" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="G14" s="7" t="n">
+        <x:v>0.631875613703866</x:v>
+      </x:c>
+      <x:c r="H14" s="8">
+        <x:v>43153</x:v>
+      </x:c>
+      <x:c r="I14" s="9" t="n">
+        <x:v>1443</x:v>
+      </x:c>
+      <x:c r="J14" s="5" t="n">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="K14" s="5" t="n">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="L14" s="5" t="s"/>
+      <x:c r="M14" s="5" t="s"/>
+      <x:c r="N14" s="5" t="s"/>
+    </x:row>
+    <x:row r="15" spans="1:14">
+      <x:c r="A15" s="5" t="n">
+        <x:v>4295904562</x:v>
+      </x:c>
+      <x:c r="B15" s="5" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="C15" s="5" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="D15" s="5" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="E15" s="5" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="F15" s="5" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="G15" s="7" t="n">
+        <x:v>0.633935468899661</x:v>
+      </x:c>
+      <x:c r="H15" s="8">
+        <x:v>42677</x:v>
+      </x:c>
+      <x:c r="I15" s="9" t="n">
+        <x:v>1919</x:v>
+      </x:c>
+      <x:c r="J15" s="5" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="K15" s="5" t="n">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="L15" s="5" t="n">
+        <x:v>7414000000</x:v>
+      </x:c>
+      <x:c r="M15" s="5" t="n">
+        <x:v>88</x:v>
+      </x:c>
+      <x:c r="N15" s="5" t="s">
+        <x:v>44</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:14">
+      <x:c r="A16" s="5" t="n">
+        <x:v>4295882004</x:v>
+      </x:c>
+      <x:c r="B16" s="5" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="C16" s="5" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="D16" s="5" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="E16" s="5" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="F16" s="5" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="G16" s="7" t="n">
+        <x:v>0.610303153850304</x:v>
+      </x:c>
+      <x:c r="H16" s="8">
+        <x:v>42979</x:v>
+      </x:c>
+      <x:c r="I16" s="9" t="n">
+        <x:v>1617</x:v>
+      </x:c>
+      <x:c r="J16" s="5" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="K16" s="5" t="n">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="L16" s="5" t="n">
+        <x:v>25541366903.8192</x:v>
+      </x:c>
+      <x:c r="M16" s="5" t="n">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="N16" s="5" t="s">
+        <x:v>46</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:14">
+      <x:c r="A17" s="5" t="n">
+        <x:v>4295865303</x:v>
+      </x:c>
+      <x:c r="B17" s="5" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="C17" s="5" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="D17" s="5" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="E17" s="5" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="F17" s="5" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="G17" s="7" t="n">
+        <x:v>0.568006968</x:v>
+      </x:c>
+      <x:c r="H17" s="8">
+        <x:v>44545</x:v>
+      </x:c>
+      <x:c r="I17" s="9" t="n">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="J17" s="5" t="n">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="K17" s="5" t="n">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="L17" s="5" t="n">
+        <x:v>4239917214.02205</x:v>
+      </x:c>
+      <x:c r="M17" s="5" t="n">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="N17" s="5" t="s">
+        <x:v>49</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:14">
+      <x:c r="A18" s="5" t="n">
+        <x:v>5000075491</x:v>
+      </x:c>
+      <x:c r="B18" s="5" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="C18" s="5" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="D18" s="5" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="E18" s="5" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="F18" s="5" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="G18" s="7" t="n">
+        <x:v>0.558914017152</x:v>
+      </x:c>
+      <x:c r="H18" s="8">
+        <x:v>43517</x:v>
+      </x:c>
+      <x:c r="I18" s="9" t="n">
+        <x:v>1079</x:v>
+      </x:c>
+      <x:c r="J18" s="5" t="n">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="K18" s="5" t="n">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="L18" s="5" t="n">
+        <x:v>8145725671.3854</x:v>
+      </x:c>
+      <x:c r="M18" s="5" t="n">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="N18" s="5" t="s">
+        <x:v>27</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:14">
+      <x:c r="A19" s="5" t="n">
+        <x:v>4295892065</x:v>
+      </x:c>
+      <x:c r="B19" s="5" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="C19" s="5" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="D19" s="5" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="E19" s="5" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="F19" s="5" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="G19" s="7" t="n">
+        <x:v>0.551251605504</x:v>
+      </x:c>
+      <x:c r="H19" s="8">
+        <x:v>43517</x:v>
+      </x:c>
+      <x:c r="I19" s="9" t="n">
+        <x:v>1079</x:v>
+      </x:c>
+      <x:c r="J19" s="5" t="n">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="K19" s="5" t="n">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="L19" s="5" t="n">
+        <x:v>9171410657.88415</x:v>
+      </x:c>
+      <x:c r="M19" s="5" t="n">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="N19" s="5" t="s">
+        <x:v>22</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:14">
+      <x:c r="A20" s="5" t="n">
+        <x:v>5035743844</x:v>
+      </x:c>
+      <x:c r="B20" s="5" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="C20" s="5" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="D20" s="5" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="E20" s="5" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="F20" s="5" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="G20" s="7" t="n">
+        <x:v>0.547036996224</x:v>
+      </x:c>
+      <x:c r="H20" s="8">
+        <x:v>41332</x:v>
+      </x:c>
+      <x:c r="I20" s="9" t="n">
+        <x:v>3264</x:v>
+      </x:c>
+      <x:c r="J20" s="5" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="K20" s="5" t="n">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="L20" s="5" t="s"/>
+      <x:c r="M20" s="5" t="s"/>
+      <x:c r="N20" s="5" t="s"/>
+    </x:row>
+    <x:row r="21" spans="1:14">
+      <x:c r="A21" s="5" t="n">
+        <x:v>4295869284</x:v>
+      </x:c>
+      <x:c r="B21" s="5" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="C21" s="5" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="D21" s="5" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="E21" s="5" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="F21" s="5" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="G21" s="7" t="n">
+        <x:v>0.528620653392</x:v>
+      </x:c>
+      <x:c r="H21" s="8">
+        <x:v>42979</x:v>
+      </x:c>
+      <x:c r="I21" s="9" t="n">
+        <x:v>1617</x:v>
+      </x:c>
+      <x:c r="J21" s="5" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="K21" s="5" t="n">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="L21" s="5" t="s"/>
+      <x:c r="M21" s="5" t="s"/>
+      <x:c r="N21" s="5" t="s"/>
+    </x:row>
+    <x:row r="22" spans="1:14">
+      <x:c r="A22" s="5" t="n">
+        <x:v>4296010499</x:v>
+      </x:c>
+      <x:c r="B22" s="5" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="C22" s="5" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="D22" s="5" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="E22" s="5" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="F22" s="5" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="G22" s="7" t="n">
+        <x:v>0.528620653392</x:v>
+      </x:c>
+      <x:c r="H22" s="8">
+        <x:v>43153</x:v>
+      </x:c>
+      <x:c r="I22" s="9" t="n">
+        <x:v>1443</x:v>
+      </x:c>
+      <x:c r="J22" s="5" t="n">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="K22" s="5" t="n">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="L22" s="5" t="s"/>
+      <x:c r="M22" s="5" t="s"/>
+      <x:c r="N22" s="5" t="s"/>
+    </x:row>
+    <x:row r="23" spans="1:14">
+      <x:c r="A23" s="5" t="n">
+        <x:v>4295886753</x:v>
+      </x:c>
+      <x:c r="B23" s="5" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="C23" s="5" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="D23" s="5" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="E23" s="5" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="F23" s="5" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="G23" s="7" t="n">
+        <x:v>0.534442158336</x:v>
+      </x:c>
+      <x:c r="H23" s="8">
+        <x:v>42979</x:v>
+      </x:c>
+      <x:c r="I23" s="9" t="n">
+        <x:v>1617</x:v>
+      </x:c>
+      <x:c r="J23" s="5" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="K23" s="5" t="n">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="L23" s="5" t="n">
+        <x:v>3546890.86401722</x:v>
+      </x:c>
+      <x:c r="M23" s="5" t="s"/>
+      <x:c r="N23" s="5" t="s">
+        <x:v>27</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:14">
+      <x:c r="A24" s="5" t="n">
+        <x:v>4295880409</x:v>
+      </x:c>
+      <x:c r="B24" s="5" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="C24" s="5" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="D24" s="5" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="E24" s="5" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="F24" s="5" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="G24" s="7" t="n">
+        <x:v>0.30660408</x:v>
+      </x:c>
+      <x:c r="H24" s="8">
+        <x:v>40785</x:v>
+      </x:c>
+      <x:c r="I24" s="9" t="n">
+        <x:v>3811</x:v>
+      </x:c>
+      <x:c r="J24" s="5" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="K24" s="5" t="n">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="L24" s="5" t="n">
+        <x:v>42990263289.0324</x:v>
+      </x:c>
+      <x:c r="M24" s="5" t="n">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="N24" s="5" t="s">
+        <x:v>49</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="25" spans="1:14">
+      <x:c r="A25" s="5" t="n">
+        <x:v>4295877797</x:v>
+      </x:c>
+      <x:c r="B25" s="5" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="C25" s="5" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="D25" s="5" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="E25" s="5" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="F25" s="5" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="G25" s="7" t="n">
+        <x:v>0.3069752</x:v>
+      </x:c>
+      <x:c r="H25" s="8">
+        <x:v>40785</x:v>
+      </x:c>
+      <x:c r="I25" s="9" t="n">
+        <x:v>3811</x:v>
+      </x:c>
+      <x:c r="J25" s="5" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="K25" s="5" t="n">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="L25" s="5" t="n">
+        <x:v>63200994987.2912</x:v>
+      </x:c>
+      <x:c r="M25" s="5" t="n">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="N25" s="5" t="s">
+        <x:v>46</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="26" spans="1:14">
+      <x:c r="A26" s="5" t="n">
+        <x:v>4295886753</x:v>
+      </x:c>
+      <x:c r="B26" s="5" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="C26" s="5" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="D26" s="5" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="E26" s="5" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="F26" s="5" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="G26" s="7" t="n">
+        <x:v>0.30953336</x:v>
+      </x:c>
+      <x:c r="H26" s="8">
+        <x:v>43066</x:v>
+      </x:c>
+      <x:c r="I26" s="9" t="n">
+        <x:v>1530</x:v>
+      </x:c>
+      <x:c r="J26" s="5" t="n">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="K26" s="5" t="n">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="L26" s="5" t="n">
+        <x:v>3546890.86401722</x:v>
+      </x:c>
+      <x:c r="M26" s="5" t="s"/>
+      <x:c r="N26" s="5" t="s">
+        <x:v>27</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27" spans="1:14">
+      <x:c r="A27" s="5" t="n">
+        <x:v>5000679258</x:v>
+      </x:c>
+      <x:c r="B27" s="5" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="C27" s="5" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="D27" s="5" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="E27" s="5" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="F27" s="5" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="G27" s="7" t="n">
+        <x:v>0.30246016</x:v>
+      </x:c>
+      <x:c r="H27" s="8">
+        <x:v>43517</x:v>
+      </x:c>
+      <x:c r="I27" s="9" t="n">
+        <x:v>1079</x:v>
+      </x:c>
+      <x:c r="J27" s="5" t="n">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="K27" s="5" t="n">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="L27" s="5" t="n">
+        <x:v>498115363.628789</x:v>
+      </x:c>
+      <x:c r="M27" s="5" t="n">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="N27" s="5" t="s">
+        <x:v>49</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28" spans="1:14">
+      <x:c r="A28" s="5" t="n">
+        <x:v>4295915019</x:v>
+      </x:c>
+      <x:c r="B28" s="5" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="C28" s="5" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="D28" s="5" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="E28" s="5" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="F28" s="5" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="G28" s="7" t="n">
+        <x:v>0.28777232</x:v>
+      </x:c>
+      <x:c r="H28" s="8">
+        <x:v>40967</x:v>
+      </x:c>
+      <x:c r="I28" s="9" t="n">
+        <x:v>3629</x:v>
+      </x:c>
+      <x:c r="J28" s="5" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="K28" s="5" t="n">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="L28" s="5" t="n">
+        <x:v>10126000</x:v>
+      </x:c>
+      <x:c r="M28" s="5" t="n">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="N28" s="5" t="s">
+        <x:v>49</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29" spans="1:14">
+      <x:c r="A29" s="5" t="n">
+        <x:v>5037062038</x:v>
+      </x:c>
+      <x:c r="B29" s="5" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="C29" s="5" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="D29" s="5" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="E29" s="5" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="F29" s="5" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="G29" s="7" t="n">
+        <x:v>0.2756856</x:v>
+      </x:c>
+      <x:c r="H29" s="8">
+        <x:v>42789</x:v>
+      </x:c>
+      <x:c r="I29" s="9" t="n">
+        <x:v>1807</x:v>
+      </x:c>
+      <x:c r="J29" s="5" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="K29" s="5" t="n">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="L29" s="5" t="n">
+        <x:v>4713210</x:v>
+      </x:c>
+      <x:c r="M29" s="5" t="s"/>
+      <x:c r="N29" s="5" t="s"/>
     </x:row>
   </x:sheetData>
   <x:mergeCells count="1">

</xml_diff>